<commit_message>
Updated Structuring Element Diagram
</commit_message>
<xml_diff>
--- a/Spreadsheet Diagrams/Methods of Crack Detection.xlsx
+++ b/Spreadsheet Diagrams/Methods of Crack Detection.xlsx
@@ -314,6 +314,255 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="676275"/>
+          <a:ext cx="285750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>A</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="1152525"/>
+          <a:ext cx="285750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>B</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="1714500"/>
+          <a:ext cx="285750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>C</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="571500" y="1990725"/>
+          <a:ext cx="285750" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>D</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -605,7 +854,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.42578125" defaultRowHeight="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1172,6 +1423,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>